<commit_message>
updated on completion of networks
</commit_message>
<xml_diff>
--- a/Assignment/Chennai  Batch - Assessment 1.xlsx
+++ b/Assignment/Chennai  Batch - Assessment 1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A98DADD-68CA-4758-809B-5A28D91DCFB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA58AC5F-C67C-48AE-BDF9-D5BA7261BA99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{8EFF61A4-5F45-4265-8801-29DDDD04C64C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{8EFF61A4-5F45-4265-8801-29DDDD04C64C}"/>
   </bookViews>
   <sheets>
     <sheet name="Attendance" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="93">
   <si>
     <t>Full Name</t>
   </si>
@@ -275,9 +275,6 @@
   </si>
   <si>
     <t>https://github.com/Lakshmiswayampakula/Fidelity-Assignments-/tree/main/src</t>
-  </si>
-  <si>
-    <t>Uploaded .class files?</t>
   </si>
   <si>
     <t>Day 6(Oct-07)</t>
@@ -460,7 +457,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -510,9 +507,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -867,23 +861,23 @@
       <c r="F1" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="G1" s="20" t="s">
         <v>70</v>
       </c>
       <c r="H1" s="15" t="s">
         <v>71</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J1" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="K1" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="L1" s="15" t="s">
         <v>85</v>
-      </c>
-      <c r="L1" s="15" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
@@ -917,10 +911,10 @@
       <c r="J2" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="K2" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="L2" s="22" t="s">
+      <c r="K2" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="L2" s="21" t="s">
         <v>63</v>
       </c>
     </row>
@@ -955,10 +949,10 @@
       <c r="J3" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="K3" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="L3" s="22" t="s">
+      <c r="K3" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="L3" s="21" t="s">
         <v>63</v>
       </c>
     </row>
@@ -993,10 +987,10 @@
       <c r="J4" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="K4" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="L4" s="22" t="s">
+      <c r="K4" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="L4" s="21" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1031,10 +1025,10 @@
       <c r="J5" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="K5" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="L5" s="22" t="s">
+      <c r="K5" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="L5" s="21" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1069,10 +1063,10 @@
       <c r="J6" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="K6" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="L6" s="22" t="s">
+      <c r="K6" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="L6" s="21" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1107,10 +1101,10 @@
       <c r="J7" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="K7" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="L7" s="22" t="s">
+      <c r="K7" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="L7" s="21" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1145,10 +1139,10 @@
       <c r="J8" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="K8" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="L8" s="22" t="s">
+      <c r="K8" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="L8" s="21" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1183,10 +1177,10 @@
       <c r="J9" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="K9" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="L9" s="22" t="s">
+      <c r="K9" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="L9" s="21" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1221,10 +1215,10 @@
       <c r="J10" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="K10" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="L10" s="22" t="s">
+      <c r="K10" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="L10" s="21" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1259,10 +1253,10 @@
       <c r="J11" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="K11" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="L11" s="22" t="s">
+      <c r="K11" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="L11" s="21" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1297,10 +1291,10 @@
       <c r="J12" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="K12" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="L12" s="22" t="s">
+      <c r="K12" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="L12" s="21" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1335,10 +1329,10 @@
       <c r="J13" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="K13" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="L13" s="22" t="s">
+      <c r="K13" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="L13" s="21" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1373,10 +1367,10 @@
       <c r="J14" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="K14" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="L14" s="22" t="s">
+      <c r="K14" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="L14" s="21" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1411,10 +1405,10 @@
       <c r="J15" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="K15" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="L15" s="22" t="s">
+      <c r="K15" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="L15" s="21" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1449,10 +1443,10 @@
       <c r="J16" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="K16" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="L16" s="22" t="s">
+      <c r="K16" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="L16" s="21" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1487,10 +1481,10 @@
       <c r="J17" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="K17" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="L17" s="22" t="s">
+      <c r="K17" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="L17" s="21" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1525,10 +1519,10 @@
       <c r="J18" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="K18" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="L18" s="22" t="s">
+      <c r="K18" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="L18" s="21" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1563,10 +1557,10 @@
       <c r="J19" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="K19" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="L19" s="22" t="s">
+      <c r="K19" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="L19" s="21" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1601,10 +1595,10 @@
       <c r="J20" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="K20" s="22" t="s">
-        <v>58</v>
-      </c>
-      <c r="L20" s="22" t="s">
+      <c r="K20" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="L20" s="21" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1618,8 +1612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBEB644E-1C8B-4219-82CB-60E92267245E}">
   <dimension ref="A1:M20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E3" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+    <sheetView topLeftCell="E3" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1660,19 +1654,19 @@
         <v>74</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J1" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="K1" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="L1" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="K1" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="L1" s="17" t="s">
+      <c r="M1" s="17" t="s">
         <v>90</v>
-      </c>
-      <c r="M1" s="17" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
@@ -1713,7 +1707,7 @@
         <v>60</v>
       </c>
       <c r="M2" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.35">
@@ -1868,7 +1862,7 @@
         <v>60</v>
       </c>
       <c r="J6" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K6" t="s">
         <v>60</v>
@@ -1877,7 +1871,7 @@
         <v>60</v>
       </c>
       <c r="M6" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.35">
@@ -1891,7 +1885,7 @@
         <v>23</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>61</v>
@@ -1900,25 +1894,25 @@
         <v>60</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I7" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J7" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K7" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="L7" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="M7" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.35">
@@ -1959,7 +1953,7 @@
         <v>60</v>
       </c>
       <c r="M8" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.35">
@@ -1999,7 +1993,7 @@
       <c r="L9" t="s">
         <v>60</v>
       </c>
-      <c r="M9" s="23" t="s">
+      <c r="M9" s="22" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2040,7 +2034,7 @@
       <c r="L10" t="s">
         <v>60</v>
       </c>
-      <c r="M10" s="23" t="s">
+      <c r="M10" s="22" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2081,8 +2075,8 @@
       <c r="L11" t="s">
         <v>60</v>
       </c>
-      <c r="M11" s="23" t="s">
-        <v>92</v>
+      <c r="M11" s="18" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.35">
@@ -2095,19 +2089,19 @@
       <c r="C12" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="F12" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="G12" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="H12" s="18" t="s">
+      <c r="D12" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G12" t="s">
+        <v>60</v>
+      </c>
+      <c r="H12" t="s">
         <v>60</v>
       </c>
       <c r="I12" t="s">
@@ -2118,6 +2112,12 @@
       </c>
       <c r="K12" t="s">
         <v>60</v>
+      </c>
+      <c r="L12" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="M12" s="18" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.35">
@@ -2145,6 +2145,21 @@
       <c r="H13" t="s">
         <v>60</v>
       </c>
+      <c r="I13" t="s">
+        <v>60</v>
+      </c>
+      <c r="J13" t="s">
+        <v>60</v>
+      </c>
+      <c r="K13" t="s">
+        <v>60</v>
+      </c>
+      <c r="L13" t="s">
+        <v>60</v>
+      </c>
+      <c r="M13" s="22" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="14" spans="1:13" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="8">
@@ -2171,6 +2186,21 @@
       <c r="H14" t="s">
         <v>60</v>
       </c>
+      <c r="I14" t="s">
+        <v>60</v>
+      </c>
+      <c r="J14" t="s">
+        <v>60</v>
+      </c>
+      <c r="K14" t="s">
+        <v>60</v>
+      </c>
+      <c r="L14" t="s">
+        <v>60</v>
+      </c>
+      <c r="M14" s="22" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15" s="8">
@@ -2185,16 +2215,16 @@
       <c r="D15" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E15" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>60</v>
-      </c>
-      <c r="G15" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="H15" s="18" t="s">
+      <c r="E15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15" t="s">
+        <v>60</v>
+      </c>
+      <c r="H15" t="s">
         <v>60</v>
       </c>
       <c r="I15" t="s">
@@ -2205,6 +2235,12 @@
       </c>
       <c r="K15" t="s">
         <v>60</v>
+      </c>
+      <c r="L15" t="s">
+        <v>60</v>
+      </c>
+      <c r="M15" s="18" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.35">
@@ -2241,8 +2277,14 @@
       <c r="K16" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L16" t="s">
+        <v>60</v>
+      </c>
+      <c r="M16" s="22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="8">
         <v>16</v>
       </c>
@@ -2276,8 +2318,14 @@
       <c r="K17" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L17" t="s">
+        <v>60</v>
+      </c>
+      <c r="M17" s="22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="8">
         <v>17</v>
       </c>
@@ -2305,8 +2353,20 @@
       <c r="I18" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="J18" t="s">
+        <v>60</v>
+      </c>
+      <c r="K18" t="s">
+        <v>60</v>
+      </c>
+      <c r="L18" t="s">
+        <v>60</v>
+      </c>
+      <c r="M18" s="22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19" s="8">
         <v>18</v>
       </c>
@@ -2331,8 +2391,23 @@
       <c r="H19" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="I19" t="s">
+        <v>60</v>
+      </c>
+      <c r="J19" t="s">
+        <v>91</v>
+      </c>
+      <c r="K19" t="s">
+        <v>60</v>
+      </c>
+      <c r="L19" t="s">
+        <v>60</v>
+      </c>
+      <c r="M19" s="18" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="8">
         <v>19</v>
       </c>
@@ -2355,6 +2430,21 @@
         <v>60</v>
       </c>
       <c r="H20" t="s">
+        <v>60</v>
+      </c>
+      <c r="I20" t="s">
+        <v>60</v>
+      </c>
+      <c r="J20" t="s">
+        <v>60</v>
+      </c>
+      <c r="K20" t="s">
+        <v>60</v>
+      </c>
+      <c r="L20" t="s">
+        <v>60</v>
+      </c>
+      <c r="M20" s="22" t="s">
         <v>60</v>
       </c>
     </row>
@@ -2387,8 +2477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26313228-B4F7-4731-9C54-5A2ECFFA97CF}">
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView topLeftCell="C3" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2423,10 +2513,10 @@
         <v>75</v>
       </c>
       <c r="H1" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" s="12" t="s">
         <v>82</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
@@ -2445,10 +2535,10 @@
       <c r="E2" s="5">
         <v>65</v>
       </c>
-      <c r="F2">
-        <v>65</v>
-      </c>
-      <c r="G2">
+      <c r="F2" s="3">
+        <v>65</v>
+      </c>
+      <c r="G2" s="3">
         <v>65</v>
       </c>
     </row>
@@ -2468,10 +2558,10 @@
       <c r="E3" s="5">
         <v>64</v>
       </c>
-      <c r="F3">
-        <v>65</v>
-      </c>
-      <c r="G3">
+      <c r="F3" s="3">
+        <v>65</v>
+      </c>
+      <c r="G3" s="3">
         <v>65</v>
       </c>
     </row>
@@ -2491,10 +2581,10 @@
       <c r="E4" s="5">
         <v>65</v>
       </c>
-      <c r="F4">
-        <v>65</v>
-      </c>
-      <c r="G4">
+      <c r="F4" s="3">
+        <v>65</v>
+      </c>
+      <c r="G4" s="3">
         <v>65</v>
       </c>
     </row>
@@ -2514,10 +2604,10 @@
       <c r="E5" s="5">
         <v>65</v>
       </c>
-      <c r="F5">
-        <v>65</v>
-      </c>
-      <c r="G5">
+      <c r="F5" s="3">
+        <v>65</v>
+      </c>
+      <c r="G5" s="3">
         <v>65</v>
       </c>
     </row>
@@ -2537,10 +2627,10 @@
       <c r="E6" s="5">
         <v>65</v>
       </c>
-      <c r="F6">
-        <v>60</v>
-      </c>
-      <c r="G6">
+      <c r="F6" s="3">
+        <v>60</v>
+      </c>
+      <c r="G6" s="3">
         <v>65</v>
       </c>
     </row>
@@ -2555,10 +2645,17 @@
         <v>23</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="E7" s="19"/>
-      <c r="F7" s="18"/>
+        <v>86</v>
+      </c>
+      <c r="E7" s="3">
+        <v>58</v>
+      </c>
+      <c r="F7" s="3">
+        <v>60</v>
+      </c>
+      <c r="G7" s="3">
+        <v>60</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="8">
@@ -2576,10 +2673,10 @@
       <c r="E8" s="5">
         <v>65</v>
       </c>
-      <c r="F8">
-        <v>65</v>
-      </c>
-      <c r="G8">
+      <c r="F8" s="3">
+        <v>65</v>
+      </c>
+      <c r="G8" s="3">
         <v>65</v>
       </c>
     </row>
@@ -2599,10 +2696,10 @@
       <c r="E9" s="5">
         <v>65</v>
       </c>
-      <c r="F9">
-        <v>60</v>
-      </c>
-      <c r="G9">
+      <c r="F9" s="3">
+        <v>60</v>
+      </c>
+      <c r="G9" s="3">
         <v>65</v>
       </c>
     </row>
@@ -2622,10 +2719,10 @@
       <c r="E10" s="5">
         <v>67</v>
       </c>
-      <c r="F10">
-        <v>65</v>
-      </c>
-      <c r="G10">
+      <c r="F10" s="3">
+        <v>65</v>
+      </c>
+      <c r="G10" s="3">
         <v>65</v>
       </c>
     </row>
@@ -2645,10 +2742,10 @@
       <c r="E11" s="5">
         <v>64</v>
       </c>
-      <c r="F11">
-        <v>65</v>
-      </c>
-      <c r="G11">
+      <c r="F11" s="3">
+        <v>65</v>
+      </c>
+      <c r="G11" s="3">
         <v>65</v>
       </c>
     </row>
@@ -2663,15 +2760,15 @@
         <v>37</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E12" s="19">
-        <v>63</v>
-      </c>
-      <c r="F12" s="18">
-        <v>65</v>
-      </c>
-      <c r="G12">
+        <v>80</v>
+      </c>
+      <c r="E12" s="5">
+        <v>63</v>
+      </c>
+      <c r="F12" s="5">
+        <v>65</v>
+      </c>
+      <c r="G12" s="3">
         <v>63</v>
       </c>
     </row>
@@ -2691,10 +2788,10 @@
       <c r="E13" s="5">
         <v>65</v>
       </c>
-      <c r="F13">
-        <v>63</v>
-      </c>
-      <c r="G13">
+      <c r="F13" s="3">
+        <v>63</v>
+      </c>
+      <c r="G13" s="3">
         <v>65</v>
       </c>
     </row>
@@ -2714,10 +2811,10 @@
       <c r="E14" s="5">
         <v>65</v>
       </c>
-      <c r="F14">
-        <v>63</v>
-      </c>
-      <c r="G14">
+      <c r="F14" s="3">
+        <v>63</v>
+      </c>
+      <c r="G14" s="3">
         <v>65</v>
       </c>
     </row>
@@ -2737,10 +2834,10 @@
       <c r="E15" s="5">
         <v>65</v>
       </c>
-      <c r="F15">
-        <v>63</v>
-      </c>
-      <c r="G15">
+      <c r="F15" s="3">
+        <v>63</v>
+      </c>
+      <c r="G15" s="3">
         <v>63</v>
       </c>
     </row>
@@ -2760,10 +2857,10 @@
       <c r="E16" s="5">
         <v>65</v>
       </c>
-      <c r="F16">
-        <v>63</v>
-      </c>
-      <c r="G16">
+      <c r="F16" s="3">
+        <v>63</v>
+      </c>
+      <c r="G16" s="3">
         <v>63</v>
       </c>
     </row>
@@ -2783,10 +2880,10 @@
       <c r="E17" s="5">
         <v>65</v>
       </c>
-      <c r="F17">
-        <v>63</v>
-      </c>
-      <c r="G17">
+      <c r="F17" s="3">
+        <v>63</v>
+      </c>
+      <c r="G17" s="3">
         <v>65</v>
       </c>
     </row>
@@ -2806,10 +2903,10 @@
       <c r="E18" s="5">
         <v>63</v>
       </c>
-      <c r="F18" t="s">
-        <v>79</v>
-      </c>
-      <c r="G18">
+      <c r="F18" s="3">
+        <v>63</v>
+      </c>
+      <c r="G18" s="3">
         <v>63</v>
       </c>
     </row>
@@ -2829,10 +2926,10 @@
       <c r="E19" s="5">
         <v>60</v>
       </c>
-      <c r="F19" s="18">
-        <v>58</v>
-      </c>
-      <c r="G19">
+      <c r="F19" s="3">
+        <v>58</v>
+      </c>
+      <c r="G19" s="3">
         <v>63</v>
       </c>
     </row>
@@ -2852,10 +2949,10 @@
       <c r="E20" s="5">
         <v>64</v>
       </c>
-      <c r="F20">
-        <v>65</v>
-      </c>
-      <c r="G20">
+      <c r="F20" s="3">
+        <v>65</v>
+      </c>
+      <c r="G20" s="3">
         <v>65</v>
       </c>
     </row>

</xml_diff>